<commit_message>
Iterates through stl files in a folder
</commit_message>
<xml_diff>
--- a/CAD Database Creation Tool/CAD Database Creation Tool/ReverseEngineeringTests.xlsx
+++ b/CAD Database Creation Tool/CAD Database Creation Tool/ReverseEngineeringTests.xlsx
@@ -14,33 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>bPart Name</t>
-  </si>
-  <si>
-    <t>Part Volume</t>
-  </si>
-  <si>
-    <t>Bounding Box Volume</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>X Length</t>
-  </si>
-  <si>
-    <t>Y Length</t>
-  </si>
-  <si>
-    <t>Surface Area</t>
-  </si>
-  <si>
-    <t>Bottom Area</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>FRAME 1.stl</t>
+  </si>
+  <si>
+    <t>jug.stl</t>
+  </si>
+  <si>
+    <t>Leo.stl</t>
+  </si>
+  <si>
+    <t>LoLtreasurev02.stl</t>
+  </si>
+  <si>
+    <t>PlasticBottle.stl</t>
   </si>
   <si>
     <t>scew_model_test.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.05.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.1.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.15.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.2.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.25.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.27.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.3.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.33.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.4.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.5.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.6.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.67.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.8.stl</t>
+  </si>
+  <si>
+    <t>scew_model_test_.9.stl</t>
+  </si>
+  <si>
+    <t>waterPump.stl</t>
   </si>
 </sst>
 </file>
@@ -372,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -382,52 +418,546 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
+      <c r="B1">
+        <v>131293.2327803425</v>
+      </c>
+      <c r="C1">
+        <v>439040</v>
+      </c>
+      <c r="D1">
+        <v>35</v>
+      </c>
+      <c r="E1">
+        <v>112</v>
+      </c>
+      <c r="F1">
+        <v>112</v>
+      </c>
+      <c r="G1">
+        <v>37330.79193073035</v>
+      </c>
+      <c r="H1">
+        <v>12544</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1691.291561640925</v>
+      </c>
+      <c r="C2">
+        <v>136142.9772500462</v>
+      </c>
+      <c r="D2">
+        <v>54.35069847106934</v>
+      </c>
+      <c r="E2">
+        <v>59.8774995803833</v>
+      </c>
+      <c r="F2">
+        <v>41.83371734619141</v>
+      </c>
+      <c r="G2">
+        <v>15744.07744370512</v>
+      </c>
+      <c r="H2">
+        <v>2504.89839284245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>46468133.26706824</v>
+      </c>
+      <c r="C4">
+        <v>247868670.3538724</v>
+      </c>
+      <c r="D4">
+        <v>1030.426845468581</v>
+      </c>
+      <c r="E4">
+        <v>385.8899688720703</v>
+      </c>
+      <c r="F4">
+        <v>623.3629455566406</v>
+      </c>
+      <c r="G4">
+        <v>1620290.84981412</v>
+      </c>
+      <c r="H4">
+        <v>240549.5076568541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>50350.07114816874</v>
+      </c>
+      <c r="C7">
+        <v>171986.4360578173</v>
+      </c>
+      <c r="D7">
+        <v>56.09999847412109</v>
+      </c>
+      <c r="E7">
+        <v>52.67546463012695</v>
+      </c>
+      <c r="F7">
+        <v>58.19999837875366</v>
+      </c>
+      <c r="G7">
+        <v>26966.334301051</v>
+      </c>
+      <c r="H7">
+        <v>3065.711956073485</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>350886.1602802682</v>
+      </c>
+      <c r="C9">
+        <v>12063966.08873647</v>
+      </c>
+      <c r="D9">
+        <v>125.6901550292969</v>
+      </c>
+      <c r="E9">
+        <v>276.9418792724609</v>
+      </c>
+      <c r="F9">
+        <v>346.5773773193359</v>
+      </c>
+      <c r="G9">
+        <v>450771.5386529238</v>
+      </c>
+      <c r="H9">
+        <v>95981.79018813767</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>287274.7101853613</v>
+      </c>
+      <c r="C10">
+        <v>994778.0624718696</v>
+      </c>
+      <c r="D10">
+        <v>99.49747467041016</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>99.98023223876953</v>
+      </c>
+      <c r="G10">
+        <v>31530.1999097709</v>
+      </c>
+      <c r="H10">
+        <v>9998.023223876953</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>34.81941174655806</v>
+      </c>
+      <c r="C12">
+        <v>124.3718445301056</v>
+      </c>
+      <c r="D12">
+        <v>4.974873781204224</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>77.76954653318438</v>
+      </c>
+      <c r="H12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>281.5542542359444</v>
+      </c>
+      <c r="C14">
+        <v>993.0114247625943</v>
+      </c>
+      <c r="D14">
+        <v>9.949747562408447</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>9.980267524719238</v>
+      </c>
+      <c r="G14">
+        <v>312.4816633545896</v>
+      </c>
+      <c r="H14">
+        <v>99.80267524719238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>287274.7101853613</v>
-      </c>
-      <c r="C2">
-        <v>994778.0624718696</v>
-      </c>
-      <c r="D2">
-        <v>99.49747467041016</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>99.98023223876953</v>
-      </c>
-      <c r="G2">
-        <v>31530.1999097709</v>
-      </c>
-      <c r="H2">
-        <v>9998.023223876953</v>
+      <c r="B16">
+        <v>956.6297567888092</v>
+      </c>
+      <c r="C16">
+        <v>3353.729642617154</v>
+      </c>
+      <c r="D16">
+        <v>14.92462110519409</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>14.98074722290039</v>
+      </c>
+      <c r="G16">
+        <v>705.5259018910456</v>
+      </c>
+      <c r="H16">
+        <v>224.7112083435059</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>2279.687409587514</v>
+      </c>
+      <c r="C18">
+        <v>7959.798049926758</v>
+      </c>
+      <c r="D18">
+        <v>19.89949512481689</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <v>1256.921111356592</v>
+      </c>
+      <c r="H18">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>4456.588203935825</v>
+      </c>
+      <c r="C20">
+        <v>15546.48041725159</v>
+      </c>
+      <c r="D20">
+        <v>24.87436866760254</v>
+      </c>
+      <c r="E20">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>25</v>
+      </c>
+      <c r="G20">
+        <v>1964.926861406942</v>
+      </c>
+      <c r="H20">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>5620.93498220814</v>
+      </c>
+      <c r="C22">
+        <v>19569.71626105188</v>
+      </c>
+      <c r="D22">
+        <v>26.86431789398193</v>
+      </c>
+      <c r="E22">
+        <v>27</v>
+      </c>
+      <c r="F22">
+        <v>26.98018646240234</v>
+      </c>
+      <c r="G22">
+        <v>2292.606655502997</v>
+      </c>
+      <c r="H22">
+        <v>728.4650344848633</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>7714.080748821543</v>
+      </c>
+      <c r="C24">
+        <v>26864.31798934937</v>
+      </c>
+      <c r="D24">
+        <v>29.84924221038818</v>
+      </c>
+      <c r="E24">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <v>30</v>
+      </c>
+      <c r="G24">
+        <v>2831.08226694326</v>
+      </c>
+      <c r="H24">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>10278.13713234157</v>
+      </c>
+      <c r="C26">
+        <v>35673.05153032648</v>
+      </c>
+      <c r="D26">
+        <v>32.83416748046875</v>
+      </c>
+      <c r="E26">
+        <v>33</v>
+      </c>
+      <c r="F26">
+        <v>32.92306900024414</v>
+      </c>
+      <c r="G26">
+        <v>3426.953923266994</v>
+      </c>
+      <c r="H26">
+        <v>1086.461277008057</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>18324.61568010825</v>
+      </c>
+      <c r="C28">
+        <v>63552.73118480603</v>
+      </c>
+      <c r="D28">
+        <v>39.79899024963379</v>
+      </c>
+      <c r="E28">
+        <v>40</v>
+      </c>
+      <c r="F28">
+        <v>39.92107009887695</v>
+      </c>
+      <c r="G28">
+        <v>5038.472058637341</v>
+      </c>
+      <c r="H28">
+        <v>1596.842803955078</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>35826.44822405747</v>
+      </c>
+      <c r="C30">
+        <v>124371.8433380127</v>
+      </c>
+      <c r="D30">
+        <v>49.74873733520508</v>
+      </c>
+      <c r="E30">
+        <v>50</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>7875.819734146831</v>
+      </c>
+      <c r="H30">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>61950.82762843699</v>
+      </c>
+      <c r="C32">
+        <v>214843.2866829862</v>
+      </c>
+      <c r="D32">
+        <v>59.69848442077637</v>
+      </c>
+      <c r="E32">
+        <v>60</v>
+      </c>
+      <c r="F32">
+        <v>59.98010635375977</v>
+      </c>
+      <c r="G32">
+        <v>11343.79807751533</v>
+      </c>
+      <c r="H32">
+        <v>3598.806381225586</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>86304.7603554067</v>
+      </c>
+      <c r="C34">
+        <v>299164.214483524</v>
+      </c>
+      <c r="D34">
+        <v>66.66330718994141</v>
+      </c>
+      <c r="E34">
+        <v>67</v>
+      </c>
+      <c r="F34">
+        <v>66.98043823242188</v>
+      </c>
+      <c r="G34">
+        <v>14147.7536170713</v>
+      </c>
+      <c r="H34">
+        <v>4487.689361572266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>147022.2427426623</v>
+      </c>
+      <c r="C36">
+        <v>509302.4118542718</v>
+      </c>
+      <c r="D36">
+        <v>79.59798049926758</v>
+      </c>
+      <c r="E36">
+        <v>80</v>
+      </c>
+      <c r="F36">
+        <v>79.98042297363281</v>
+      </c>
+      <c r="G36">
+        <v>20176.45317818065</v>
+      </c>
+      <c r="H36">
+        <v>6398.433837890625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38">
+        <v>209399.100684967</v>
+      </c>
+      <c r="C38">
+        <v>725177.5097124521</v>
+      </c>
+      <c r="D38">
+        <v>89.54772567749023</v>
+      </c>
+      <c r="E38">
+        <v>90</v>
+      </c>
+      <c r="F38">
+        <v>89.98026275634766</v>
+      </c>
+      <c r="G38">
+        <v>25538.39649012632</v>
+      </c>
+      <c r="H38">
+        <v>8098.223648071289</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>131355.3442284274</v>
+      </c>
+      <c r="C40">
+        <v>672095.6663593358</v>
+      </c>
+      <c r="D40">
+        <v>41.38063430786133</v>
+      </c>
+      <c r="E40">
+        <v>143.6531867980957</v>
+      </c>
+      <c r="F40">
+        <v>113.0625267028809</v>
+      </c>
+      <c r="G40">
+        <v>36109.07695691389</v>
+      </c>
+      <c r="H40">
+        <v>16241.79226831363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>